<commit_message>
Auto-committed on 2023/01/18 週三 11:41:41.81
</commit_message>
<xml_diff>
--- a/Program/Other/L9133_底稿_會計與主檔餘額檢核表.xlsx
+++ b/Program/Other/L9133_底稿_會計與主檔餘額檢核表.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34B2FBB-EB21-4DD2-A311-84CE340C1F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38C03C4-D9AF-4C70-ABC3-C623A4860C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="檢核表" sheetId="1" r:id="rId1"/>
-    <sheet name="未銷帳" sheetId="3" r:id="rId2"/>
+    <sheet name="應收應付" sheetId="5" r:id="rId2"/>
+    <sheet name="未銷帳" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>區隔帳冊</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -423,11 +424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CD5734-99F4-4209-97BC-5EC8E580EFF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C342989-13AD-40D2-84B0-56338C3623D5}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -464,4 +465,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CD5734-99F4-4209-97BC-5EC8E580EFF3}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="24.625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="30.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2023/02/09 週四 17:32:45.66
</commit_message>
<xml_diff>
--- a/Program/Other/L9133_底稿_會計與主檔餘額檢核表.xlsx
+++ b/Program/Other/L9133_底稿_會計與主檔餘額檢核表.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38C03C4-D9AF-4C70-ABC3-C623A4860C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="檢核表" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>區隔帳冊</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,12 +53,28 @@
   </si>
   <si>
     <t>銷帳檔與主檔差額</t>
+  </si>
+  <si>
+    <t>前日餘額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>減</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淨增減</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,20 +395,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="24.59765625" defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="30.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,15 +419,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -424,20 +451,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C342989-13AD-40D2-84B0-56338C3623D5}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="24.59765625" defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="30.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,15 +475,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -468,20 +507,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CD5734-99F4-4209-97BC-5EC8E580EFF3}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="24.59765625" defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="30.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,18 +528,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>